<commit_message>
Se modifica layout para actualziar SDI
</commit_message>
<xml_diff>
--- a/TadaNomina/Formatos/ActualizacionSDI.xlsx
+++ b/TadaNomina/Formatos/ActualizacionSDI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\Documents\AzureDevOps\TadaNomina\TadaNomina\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B837A379-CBD6-47FD-B55A-B034F9AC792E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B32D5A4-4DDA-455D-BD95-5F425FB11F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C2C24A70-CC51-49D5-A96A-A31830415AFF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C2C24A70-CC51-49D5-A96A-A31830415AFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Información" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <t>12555578901</t>
   </si>
   <si>
-    <t>Tipo de salario que se asignará ante IMSS, generalmente es 1</t>
+    <t>Tipo de salario que se asignará ante IMSS: 0 (CERO) Salario fijo, 1 (UNO) Salario variable, 2 (DOS) Salario mixto</t>
   </si>
 </sst>
 </file>
@@ -201,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,6 +222,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
@@ -539,7 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E535C6-AFE3-4FAC-897E-775B3F120CB9}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -615,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393E5222-FA00-4861-8CE7-20B81F1C93FC}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,7 +744,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -757,7 +760,7 @@
       <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="10" t="s">
         <v>25</v>
       </c>
       <c r="G6">

</xml_diff>